<commit_message>
Add docker image hashes in README.md
</commit_message>
<xml_diff>
--- a/resources/scripts/rougeEvaluation/GoldFileInformationOut.xlsx
+++ b/resources/scripts/rougeEvaluation/GoldFileInformationOut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calga\Documents\gitHubRepos\CodeRepo\resources\scripts\rougeEvaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6620ADA3-3ACF-4EA1-B244-B967BEDA94E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AF8863-D39D-4CA7-8DBF-A544A436202C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="709" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="709" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtractedSentences" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,20 @@
     <sheet name="rouge_2" sheetId="10" r:id="rId10"/>
     <sheet name="rouge_l" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2211,6 +2224,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2308,7 +2324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2320,7 +2336,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2328,10 +2343,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2499,7 +2516,7 @@
             <c:numRef>
               <c:f>rouge_1!$A$2:$A$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>6.3452160922941786E-2</c:v>
@@ -2611,7 +2628,7 @@
             <c:numRef>
               <c:f>rouge_1!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.1497067969917509E-2</c:v>
@@ -2722,7 +2739,7 @@
             <c:numRef>
               <c:f>rouge_1!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3.2114132970388433E-2</c:v>
@@ -2834,7 +2851,7 @@
             <c:numRef>
               <c:f>rouge_1!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.384615228777425E-2</c:v>
@@ -2946,7 +2963,7 @@
             <c:numRef>
               <c:f>rouge_1!$E$2:$E$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>6.8321243452411459E-2</c:v>
@@ -3057,7 +3074,7 @@
             <c:numRef>
               <c:f>rouge_1!$F$2:$F$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>6.0226152111033847E-2</c:v>
@@ -3238,7 +3255,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3506,7 +3523,7 @@
             <c:numRef>
               <c:f>rouge_2!$A$2:$A$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.0633439865242501E-2</c:v>
@@ -3618,7 +3635,7 @@
             <c:numRef>
               <c:f>rouge_2!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>7.6863598392616127E-3</c:v>
@@ -3729,7 +3746,7 @@
             <c:numRef>
               <c:f>rouge_2!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>8.9228535739185634E-3</c:v>
@@ -3841,7 +3858,7 @@
             <c:numRef>
               <c:f>rouge_2!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.6126120493792698E-2</c:v>
@@ -3953,7 +3970,7 @@
             <c:numRef>
               <c:f>rouge_2!$E$2:$E$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.6423866718326231E-2</c:v>
@@ -4064,7 +4081,7 @@
             <c:numRef>
               <c:f>rouge_2!$F$2:$F$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.6273631811143139E-2</c:v>
@@ -4245,7 +4262,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4398,7 +4415,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>ROUGE-l</a:t>
+              <a:t>ROUGE-L</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -4513,7 +4530,7 @@
             <c:numRef>
               <c:f>rouge_l!$A$2:$A$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.82266738139538E-2</c:v>
@@ -4625,7 +4642,7 @@
             <c:numRef>
               <c:f>rouge_l!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.9859955444300369E-2</c:v>
@@ -4736,7 +4753,7 @@
             <c:numRef>
               <c:f>rouge_l!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.961785285392373E-2</c:v>
@@ -4848,7 +4865,7 @@
             <c:numRef>
               <c:f>rouge_l!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.2584996898626682E-2</c:v>
@@ -4960,7 +4977,7 @@
             <c:numRef>
               <c:f>rouge_l!$E$2:$E$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>6.6016432158836125E-2</c:v>
@@ -5071,7 +5088,7 @@
             <c:numRef>
               <c:f>rouge_l!$F$2:$F$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.8540169505864131E-2</c:v>
@@ -5252,7 +5269,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -10621,7 +10638,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="F11" sqref="A2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10639,249 +10656,249 @@
       <c r="B1" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>722</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>724</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="9">
         <v>1.0633439865242501E-2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="9">
         <v>7.6863598392616127E-3</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="10">
         <v>8.9228535739185634E-3</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="11">
         <v>1.6126120493792698E-2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="9">
         <v>1.6423866718326231E-2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="10">
         <v>1.6273631811143139E-2</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="9">
         <v>1.450693881428654E-2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="9">
         <v>4.8342033366346E-3</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="10">
         <v>7.2518459843942552E-3</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="11">
         <v>4.2083000080353358E-2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="9">
         <v>1.872098789865273E-2</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="10">
         <v>2.591393628705126E-2</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="9">
         <v>4.2590114355840883E-2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="9">
         <v>7.3756396388455136E-3</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="10">
         <v>1.2573785465113139E-2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="11">
         <v>5.0229067496083697E-2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="9">
         <v>1.4256748616724759E-2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="10">
         <v>2.2209634047011161E-2</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="9">
         <v>7.0720204801129422E-2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="9">
         <v>6.9858413634963628E-3</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10">
         <v>1.2715616256887011E-2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="11">
         <v>6.4441503814040277E-2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="9">
         <v>1.170736975398072E-2</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="10">
         <v>1.981488306533161E-2</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="9">
         <v>7.2852050863117149E-2</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="9">
         <v>6.2993046458623032E-3</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="10">
         <v>1.1595941964899589E-2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="11">
         <v>7.2089371121064311E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="9">
         <v>1.275054829753948E-2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="10">
         <v>2.1668549770376602E-2</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="9">
         <v>9.9215200821772723E-2</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="9">
         <v>6.1889848898719433E-3</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="10">
         <v>1.1651176366210001E-2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="11">
         <v>7.3526938782933635E-2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="9">
         <v>1.160488193732913E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="10">
         <v>2.004588734435651E-2</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>0.12557399186989271</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="9">
         <v>6.9332460346007508E-3</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="10">
         <v>1.314094829760837E-2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="11">
         <v>7.4513742997780824E-2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="9">
         <v>1.0297490835327661E-2</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="10">
         <v>1.8094409217899371E-2</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="9">
         <v>0.1592167299947195</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>8.5284259061044546E-3</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="10">
         <v>1.6189654806783419E-2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="11">
         <v>7.4513742997780824E-2</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="9">
         <v>9.2807072688508747E-3</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="10">
         <v>1.6505633346082661E-2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="9">
         <v>0.18788118626988301</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="9">
         <v>9.0896009448354839E-3</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="10">
         <v>1.7340287180493422E-2</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="11">
         <v>7.5346035964905245E-2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="9">
         <v>8.2991975514307998E-3</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="10">
         <v>1.4951518715476699E-2</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="9">
         <v>0.1969330399020407</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="9">
         <v>8.5013138083656365E-3</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="10">
         <v>1.6299022448822621E-2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="11">
         <v>7.5742769429517784E-2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="9">
         <v>7.4288226155144969E-3</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="10">
         <v>1.3530571789344741E-2</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>10</v>
       </c>
     </row>
@@ -10895,8 +10912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD33F2C0-D1B2-44EF-A630-2B7FC8A6B1A3}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10914,255 +10931,256 @@
       <c r="B1" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>722</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>724</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="9">
         <v>5.82266738139538E-2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="9">
         <v>1.9859955444300369E-2</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="10">
         <v>2.961785285392373E-2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="11">
         <v>5.2584996898626682E-2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="9">
         <v>6.6016432158836125E-2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="10">
         <v>5.8540169505864131E-2</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="9">
         <v>9.1678473528447754E-2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="9">
         <v>1.670155716199484E-2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="10">
         <v>2.8255634481838661E-2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="11">
         <v>0.10739711963805609</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="9">
         <v>5.8445954178660373E-2</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="10">
         <v>7.5697187574115463E-2</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="9">
         <v>0.14471678060281179</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="9">
         <v>1.9375164586615069E-2</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="10">
         <v>3.4174882129500282E-2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="11">
         <v>0.13699517875188669</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="9">
         <v>4.8146300495061467E-2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="10">
         <v>7.1251575491252009E-2</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="9">
         <v>0.1818159041898591</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="9">
         <v>1.796414924014407E-2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10">
         <v>3.2697639038751489E-2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="11">
         <v>0.1586953408422844</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="9">
         <v>4.0202744885386867E-2</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="10">
         <v>6.415334043101123E-2</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="9">
         <v>0.20147834530786329</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="9">
         <v>1.677067266918748E-2</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="10">
         <v>3.0963964103087049E-2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="11">
         <v>0.17582878455560691</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="9">
         <v>3.785021501511724E-2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="10">
         <v>6.229116866558243E-2</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="9">
         <v>0.2401286877586328</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="9">
         <v>1.62372382042387E-2</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="10">
         <v>3.0417667154197851E-2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="11">
         <v>0.18354711127963069</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="9">
         <v>3.4032496809402353E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="10">
         <v>5.7418675710114983E-2</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>0.28106888175746469</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="9">
         <v>1.650383785525773E-2</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="10">
         <v>3.1177019564971448E-2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="11">
         <v>0.19436957173786901</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="9">
         <v>3.0977289740877122E-2</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="10">
         <v>5.3437997769514543E-2</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="9">
         <v>0.3196540165125053</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>1.734116629153875E-2</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="10">
         <v>3.2897642096711352E-2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="11">
         <v>0.20243010884665039</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="9">
         <v>2.8445800413075251E-2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="10">
         <v>4.9882090273620408E-2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="9">
         <v>0.35380382328842341</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="9">
         <v>1.7524251425781422E-2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="10">
         <v>3.3394443226416742E-2</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="11">
         <v>0.20895306832759711</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="9">
         <v>2.577840006411403E-2</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="10">
         <v>4.5894790561137731E-2</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="9">
         <v>0.37183793514260383</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="9">
         <v>1.692839420083345E-2</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="10">
         <v>3.2382532487052147E-2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="11">
         <v>0.21594533208093811</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="9">
         <v>2.370090565501904E-2</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="10">
         <v>4.2713793386827167E-2</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13976,8 +13994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14175,8 +14193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E2BADC-8521-499B-8B3B-B4EC6D986B6D}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14194,249 +14212,249 @@
       <c r="B1" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>722</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>724</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="9">
         <v>6.3452160922941786E-2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="9">
         <v>2.1497067969917509E-2</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="10">
         <v>3.2114132970388433E-2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="11">
         <v>5.384615228777425E-2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="9">
         <v>6.8321243452411459E-2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="10">
         <v>6.0226152111033847E-2</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="9">
         <v>9.9801515305231819E-2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="9">
         <v>1.819791345988243E-2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="10">
         <v>3.0782849674721169E-2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="11">
         <v>0.11389968921139811</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="9">
         <v>6.2522304547892829E-2</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="10">
         <v>8.0729969150009642E-2</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="9">
         <v>0.1576409223078854</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="9">
         <v>2.0961449089423288E-2</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="10">
         <v>3.700266845859209E-2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="11">
         <v>0.14412633322347651</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="9">
         <v>5.1582885109098281E-2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="10">
         <v>7.5974470198216279E-2</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="9">
         <v>0.19532935153485231</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="9">
         <v>1.9318134895369422E-2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10">
         <v>3.5159030508395722E-2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="11">
         <v>0.16548601182732331</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="9">
         <v>4.2717303989044622E-2</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="10">
         <v>6.7905895210595521E-2</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="9">
         <v>0.21552373262299879</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="9">
         <v>1.795719047838111E-2</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="10">
         <v>3.3152179355076368E-2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="11">
         <v>0.18261886757858109</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="9">
         <v>3.9852639060054387E-2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="10">
         <v>6.542719942097211E-2</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="9">
         <v>0.25677845020953799</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="9">
         <v>1.7453254799675359E-2</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="10">
         <v>3.2684913062275223E-2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="11">
         <v>0.1903371943026049</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="9">
         <v>3.5704512714627677E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="10">
         <v>6.0129582843097377E-2</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>0.29740672692685582</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="9">
         <v>1.7593859890434129E-2</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="10">
         <v>3.3222365309806462E-2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="11">
         <v>0.20153375609968691</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="9">
         <v>3.238140272375719E-2</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="10">
         <v>5.5797544302129742E-2</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="9">
         <v>0.33762030362411022</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>1.8407027672346959E-2</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="10">
         <v>3.491072580818471E-2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="11">
         <v>0.20959429320846831</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="9">
         <v>2.966146346518363E-2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="10">
         <v>5.1968433754293039E-2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="9">
         <v>0.3703701015832882</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="9">
         <v>1.8432673133724941E-2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="10">
         <v>3.5117604425319048E-2</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="11">
         <v>0.21462872872898101</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="9">
         <v>2.6687263772994269E-2</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="10">
         <v>4.747181019762596E-2</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="9">
         <v>0.38825696109590052</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="9">
         <v>1.773475298268249E-2</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="10">
         <v>3.3920107529632933E-2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="11">
         <v>0.22128050899577109</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="9">
         <v>2.4403705902197509E-2</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="10">
         <v>4.3959392878895283E-2</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>10</v>
       </c>
     </row>

</xml_diff>